<commit_message>
fix missing header in generated xlsx with TS version
</commit_message>
<xml_diff>
--- a/tests/files/scenario_after_version_4_5_0.xlsx
+++ b/tests/files/scenario_after_version_4_5_0.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
@@ -407,16 +407,16 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -424,13 +424,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -438,13 +438,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -452,12 +452,26 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>